<commit_message>
removed all python > 1000
</commit_message>
<xml_diff>
--- a/results/python/python_overall.xlsx
+++ b/results/python/python_overall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A85A13F-F177-4117-AEE2-34FDA5E905F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18072A71-4F6C-4C9D-9921-55175C9B7020}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="795" windowWidth="24000" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,11 +155,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -444,7 +443,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C3" sqref="C3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,13 +511,13 @@
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>17.749833935018049</v>
+        <v>17.747660582255083</v>
       </c>
       <c r="F3" s="1">
-        <v>29.036514326488128</v>
+        <v>29.034117260006202</v>
       </c>
       <c r="G3" s="1">
-        <v>0.15604490367643917</v>
+        <v>0.15603427483907159</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>5</v>
@@ -544,19 +543,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>1295</v>
+        <v>397</v>
       </c>
       <c r="D4" s="1">
         <v>17</v>
       </c>
       <c r="E4" s="1">
-        <v>77.332389891696749</v>
+        <v>77.297221580406656</v>
       </c>
       <c r="F4" s="1">
-        <v>27.760053644251826</v>
+        <v>26.978107509501992</v>
       </c>
       <c r="G4" s="1">
-        <v>0.14918508634552002</v>
+        <v>0.14498492942212343</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>6</v>
@@ -588,13 +587,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>10.228447653429603</v>
+        <v>10.22851201478743</v>
       </c>
       <c r="F5" s="1">
-        <v>7.3360333748465685</v>
+        <v>7.3361295370529866</v>
       </c>
       <c r="G5" s="1">
-        <v>3.9424519364598599E-2</v>
+        <v>3.9425605476090586E-2</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>7</v>
@@ -677,7 +676,6 @@
       <c r="G9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="3"/>
       <c r="L9" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>